<commit_message>
Calculations of systems with partially predetermined eq. composition restored
A number of simplifications implemented in postproc section
</commit_message>
<xml_diff>
--- a/input/concentrations/ds.5p.ser/data3.xlsx
+++ b/input/concentrations/ds.5p.ser/data3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\wannabecoder\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\concentrations\ds.5p.ser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,9 +44,6 @@
     <t>eq</t>
   </si>
   <si>
-    <t>ser_num</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>series</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>3.9990000000000002E-4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
         <v>6.9979999999999999E-4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>9.7799999999999992E-4</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>1.5E-3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>1.99E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>9.8769999999999999E-4</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>8.8649999999999996E-3</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>